<commit_message>
<fix: import controller> fix error: cant save data to database
</commit_message>
<xml_diff>
--- a/App_Data/uploads/VUNG.xlsx
+++ b/App_Data/uploads/VUNG.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SQL\SQL practice\import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Haniki\SQL\tt1\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29318AE0-207A-4BED-BFA7-CF7DDD6BC23D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F2F3ADB-3FBA-4740-89A0-8C9552B6F28D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-104" yWindow="-104" windowWidth="20098" windowHeight="11396" xr2:uid="{CFAE077E-E0F3-412D-AB54-A01D0FDA7777}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{9E895559-6259-4BED-A8D6-1E58F04C1AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="VUNG" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -27,6 +38,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
+    <t>MÃ VÙNG</t>
+  </si>
+  <si>
+    <t>TÊN VÙNG</t>
+  </si>
+  <si>
     <t>V01</t>
   </si>
   <si>
@@ -61,12 +78,6 @@
   </si>
   <si>
     <t>Đồng bằng sông Cửu Long</t>
-  </si>
-  <si>
-    <t>MaVung</t>
-  </si>
-  <si>
-    <t>TenVung</t>
   </si>
 </sst>
 </file>
@@ -77,7 +88,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -170,39 +181,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -254,7 +265,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -365,13 +376,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -380,6 +384,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -444,84 +455,103 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BCEB4FA-6C4D-41E2-8AE5-830258D67394}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D459F2E-3904-4711-9281-8BB2A72F8A1A}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.54296875" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.55" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>